<commit_message>
24 commit: Implementando formula variancia e desvio padrao
</commit_message>
<xml_diff>
--- a/adulanco-formulas.xlsx
+++ b/adulanco-formulas.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\adulancoweb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{268A9614-5599-4036-819D-DE74E174A32A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F803D605-A4D3-4906-84EA-A842E333755B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9405" xr2:uid="{721A6AF0-082B-45AF-9A61-766CEAC7BA04}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabela localStorage" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -59,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
   <si>
     <t>Coletor</t>
   </si>
@@ -88,9 +89,6 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Média</t>
-  </si>
-  <si>
     <t>Col.  1</t>
   </si>
   <si>
@@ -211,29 +209,85 @@
     <t>CV peso</t>
   </si>
   <si>
-    <t>TL media / Nº colet</t>
-  </si>
-  <si>
-    <t>"=&gt; Peso total (ou média tl) dividido pela qtde de coletores</t>
-  </si>
-  <si>
-    <t>É a média (acima)</t>
-  </si>
-  <si>
     <t>ok</t>
   </si>
   <si>
     <t>não</t>
   </si>
   <si>
-    <t>Variância é o quadrado do peso total subtraindo média -&gt; Vari = (peso tl - média)^2 / qtde coletores</t>
+    <r>
+      <t xml:space="preserve">O </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>peso</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> é a</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> média das repetições</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> informadas por linha, pelo usuário</t>
+    </r>
+  </si>
+  <si>
+    <t>A média de cada linha é a somatória da repetição, divida pela qtde de repetições.</t>
+  </si>
+  <si>
+    <t>Ao somar a coluna MÉDIA, chega-se ao total. Esse total é dividido pelo numero total de coletores.</t>
+  </si>
+  <si>
+    <t>Média das rep</t>
+  </si>
+  <si>
+    <t>Media tl / Nº colet</t>
+  </si>
+  <si>
+    <t>"=&gt; Soma da coluna média, dividido pela qtde de coletores</t>
+  </si>
+  <si>
+    <t>Variância é o quadrado da repeticao(linha i) subtraindo média tl -&gt; Vari = (media da repetição da linha(i) - média total)^2 / qtde coletores</t>
+  </si>
+  <si>
+    <t>O PESO é o mesmo que a MÉDIA DAS REPETIÇÕES</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -275,6 +329,14 @@
       <color indexed="81"/>
       <name val="Segoe UI"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -401,6 +463,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>375722</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagem 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57FFB795-6964-48A8-821B-BE5376667836}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="123825" y="200025"/>
+          <a:ext cx="12443897" cy="5476875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -704,7 +815,7 @@
   <dimension ref="A1:Q40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+      <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,7 +825,8 @@
     <col min="3" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" style="5" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" customWidth="1"/>
-    <col min="8" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="3.5703125" customWidth="1"/>
     <col min="15" max="15" width="3" customWidth="1"/>
     <col min="16" max="16" width="18.5703125" bestFit="1" customWidth="1"/>
@@ -749,19 +861,19 @@
         <v>8</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="L1" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="N1" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="N1" s="16" t="s">
-        <v>49</v>
-      </c>
       <c r="P1" s="10" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -784,7 +896,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H2" s="4">
         <v>1</v>
@@ -814,7 +926,7 @@
         <v>23.66</v>
       </c>
       <c r="Q2" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -837,7 +949,7 @@
         <v>2.333333333333333</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H3" s="4">
         <v>2.333333333333333</v>
@@ -862,9 +974,6 @@
         <f>ROUND(($M3/$P$2)*100,2)</f>
         <v>14.82</v>
       </c>
-      <c r="P3" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -886,7 +995,7 @@
         <v>3.6666666666666665</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H4" s="4">
         <v>3.6666666666666665</v>
@@ -932,7 +1041,7 @@
         <v>5</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H5" s="4">
         <v>5</v>
@@ -958,7 +1067,7 @@
         <v>12.97</v>
       </c>
       <c r="P5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -981,7 +1090,7 @@
         <v>7.6666666666666661</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H6" s="4">
         <v>7.6666666666666661</v>
@@ -1027,7 +1136,7 @@
         <v>10.333333333333332</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H7" s="4">
         <v>10.333333333333332</v>
@@ -1053,7 +1162,7 @@
         <v>9.26</v>
       </c>
       <c r="P7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -1076,7 +1185,7 @@
         <v>13</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H8" s="4">
         <v>13</v>
@@ -1126,7 +1235,7 @@
         <v>20.333333333333332</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H9" s="4">
         <v>20.333333333333332</v>
@@ -1172,7 +1281,7 @@
         <v>27.666666666666664</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H10" s="4">
         <v>27.666666666666664</v>
@@ -1218,7 +1327,7 @@
         <v>35</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H11" s="4">
         <v>35</v>
@@ -1264,7 +1373,7 @@
         <v>36.5</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H12" s="4">
         <v>36.5</v>
@@ -1288,6 +1397,9 @@
       <c r="N12" s="5">
         <f t="shared" si="4"/>
         <v>8.92</v>
+      </c>
+      <c r="P12" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -1310,7 +1422,7 @@
         <v>38</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H13" s="4">
         <v>38</v>
@@ -1334,6 +1446,9 @@
       <c r="N13" s="5">
         <f t="shared" si="4"/>
         <v>9.9600000000000009</v>
+      </c>
+      <c r="P13" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
@@ -1356,7 +1471,7 @@
         <v>39.5</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H14" s="4">
         <v>39.5</v>
@@ -1380,6 +1495,9 @@
       <c r="N14" s="5">
         <f t="shared" si="4"/>
         <v>11.01</v>
+      </c>
+      <c r="P14" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
@@ -1402,7 +1520,7 @@
         <v>41</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H15" s="4">
         <v>41</v>
@@ -1448,7 +1566,7 @@
         <v>42.5</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H16" s="4">
         <v>42.5</v>
@@ -1494,7 +1612,7 @@
         <v>44</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H17" s="4">
         <v>44</v>
@@ -1518,6 +1636,9 @@
       <c r="N17" s="5">
         <f t="shared" si="4"/>
         <v>14.13</v>
+      </c>
+      <c r="P17" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -1540,7 +1661,7 @@
         <v>46</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H18" s="4">
         <v>46</v>
@@ -1586,7 +1707,7 @@
         <v>48</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H19" s="4">
         <v>48</v>
@@ -1632,7 +1753,7 @@
         <v>50</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H20" s="4">
         <v>50</v>
@@ -1679,7 +1800,7 @@
         <v>52</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H21" s="4">
         <v>52</v>
@@ -1725,7 +1846,7 @@
         <v>54</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H22" s="4">
         <v>54</v>
@@ -1771,7 +1892,7 @@
         <v>56</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H23" s="4">
         <v>56</v>
@@ -1817,7 +1938,7 @@
         <v>47.333333333333336</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H24" s="4">
         <v>47.333333333333336</v>
@@ -1863,7 +1984,7 @@
         <v>38.666666666666671</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H25" s="4">
         <v>38.666666666666671</v>
@@ -1909,7 +2030,7 @@
         <v>30</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H26" s="4">
         <v>30</v>
@@ -1955,7 +2076,7 @@
         <v>23.666666666666668</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H27" s="4">
         <v>23.666666666666668</v>
@@ -2001,7 +2122,7 @@
         <v>17.333333333333336</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H28" s="4">
         <v>17.333333333333336</v>
@@ -2047,7 +2168,7 @@
         <v>11</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H29" s="4">
         <v>11</v>
@@ -2093,7 +2214,7 @@
         <v>9</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H30" s="4">
         <v>9</v>
@@ -2139,7 +2260,7 @@
         <v>7</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H31" s="4">
         <v>7</v>
@@ -2185,7 +2306,7 @@
         <v>5</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H32" s="4">
         <v>5</v>
@@ -2231,7 +2352,7 @@
         <v>4</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H33" s="4">
         <v>4</v>
@@ -2277,7 +2398,7 @@
         <v>3</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="H34" s="4">
         <v>3</v>
@@ -2323,7 +2444,7 @@
         <v>2</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H35" s="4">
         <v>2</v>
@@ -2369,7 +2490,7 @@
         <v>1.6666666666666667</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H36" s="4">
         <v>1.6666666666666667</v>
@@ -2415,7 +2536,7 @@
         <v>1.3333333333333335</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H37" s="4">
         <v>1.3333333333333335</v>
@@ -2461,7 +2582,7 @@
         <v>1</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H38" s="4">
         <v>1</v>
@@ -2515,22 +2636,22 @@
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F40" s="5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I40" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="J40" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="L40" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="M40" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="N40" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2541,4 +2662,17 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2550E2E-1663-4337-842C-B5BCE19A2934}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>